<commit_message>
dashboar sobre relatório de vendas XBOX - versão final
</commit_message>
<xml_diff>
--- a/base_de_dados.xlsx
+++ b/base_de_dados.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\OneDrive\Documents\cursos da Dio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDF0425-BE2D-4705-AFD3-A67DD040F3E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CAE9A67-A441-471F-B806-96DDC4B2E91A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="417" firstSheet="3" activeTab="3" xr2:uid="{28DD5B76-0634-4F87-BE60-8BFA7EF2E23B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="417" firstSheet="3" activeTab="4" xr2:uid="{28DD5B76-0634-4F87-BE60-8BFA7EF2E23B}"/>
   </bookViews>
   <sheets>
-    <sheet name="A̳ssets" sheetId="1" state="hidden" r:id="rId1"/>
+    <sheet name="A̳ssets" sheetId="1" r:id="rId1"/>
     <sheet name="B̳ases" sheetId="2" state="hidden" r:id="rId2"/>
     <sheet name="C̳álculos" sheetId="3" state="hidden" r:id="rId3"/>
     <sheet name="D̳ashboard 1" sheetId="4" r:id="rId4"/>
@@ -1346,9 +1346,9 @@
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FF00FF99"/>
       <color rgb="FF22C55E"/>
       <color rgb="FF2AE6B1"/>
-      <color rgb="FF00FF99"/>
       <color rgb="FFFFFFFF"/>
       <color rgb="FFE8E6E9"/>
       <color rgb="FF5BF6A8"/>
@@ -4813,7 +4813,7 @@
           </a:p>
         </xdr:txBody>
       </xdr:sp>
-      <xdr:sp macro="" textlink="C̳álculos!G23">
+      <xdr:sp macro="" textlink="C̳álculos!G12">
         <xdr:nvSpPr>
           <xdr:cNvPr id="7" name="Retângulo: Cantos Arredondados 6">
             <a:extLst>
@@ -4858,16 +4858,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="l"/>
-            <a:r>
-              <a:rPr lang="en-US" sz="3600" b="0" i="0" u="none" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="00FF99"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-              </a:rPr>
-              <a:t>  </a:t>
-            </a:r>
-            <a:fld id="{2ADEA0F6-6D75-4818-8987-150267395C09}" type="TxLink">
+            <a:fld id="{C0DB44D4-CB04-4677-95A5-7E5830805307}" type="TxLink">
               <a:rPr lang="en-US" sz="3600" b="0" i="0" u="none" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="00FF99"/>
@@ -4875,9 +4866,9 @@
                 <a:latin typeface="Aptos Narrow"/>
               </a:rPr>
               <a:pPr algn="l"/>
-              <a:t> R$ 990,00 </a:t>
+              <a:t> R$ 2.308,00 </a:t>
             </a:fld>
-            <a:endParaRPr lang="pt-BR" sz="3600">
+            <a:endParaRPr lang="en-US" sz="3600">
               <a:solidFill>
                 <a:srgbClr val="00FF99"/>
               </a:solidFill>
@@ -4918,6 +4909,10 @@
           <a:prstGeom prst="rect">
             <a:avLst/>
           </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
         </xdr:spPr>
       </xdr:pic>
       <xdr:sp macro="" textlink="">
@@ -6027,78 +6022,6 @@
           </a:p>
         </xdr:txBody>
       </xdr:sp>
-      <xdr:sp macro="" textlink="C̳álculos!Y24">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="7" name="Retângulo: Cantos Arredondados 6">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBA526E5-651D-DBC8-650E-889357A3208E}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="3952874" y="1785939"/>
-            <a:ext cx="2812050" cy="842961"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="15000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:r>
-              <a:rPr lang="en-US" sz="3600" b="0" i="0" u="none" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="00FF99"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-              </a:rPr>
-              <a:t>  </a:t>
-            </a:r>
-            <a:fld id="{2ADEA0F6-6D75-4818-8987-150267395C09}" type="TxLink">
-              <a:rPr lang="en-US" sz="3600" b="0" i="0" u="none" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="00FF99"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-              </a:rPr>
-              <a:pPr algn="l"/>
-              <a:t> R$ 1.350,00 </a:t>
-            </a:fld>
-            <a:endParaRPr lang="pt-BR" sz="3600">
-              <a:solidFill>
-                <a:srgbClr val="00FF99"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
       <xdr:pic>
         <xdr:nvPicPr>
           <xdr:cNvPr id="8" name="Imagem 7">
@@ -6988,6 +6911,84 @@
             <a:t> R$ 1.140,00 </a:t>
           </a:fld>
           <a:endParaRPr lang="pt-BR" sz="3600">
+            <a:solidFill>
+              <a:srgbClr val="00FF99"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>589430</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>71158</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>390856</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>132428</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="C̳álculos!G12">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="Retângulo: Cantos Arredondados 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51D7AE82-DBEB-4A1B-8413-A0105A439D06}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4410636" y="2110629"/>
+          <a:ext cx="2827014" cy="823270"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:fld id="{C0DB44D4-CB04-4677-95A5-7E5830805307}" type="TxLink">
+            <a:rPr lang="en-US" sz="3600" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="00FF99"/>
+              </a:solidFill>
+              <a:latin typeface="Aptos Narrow"/>
+            </a:rPr>
+            <a:pPr algn="l"/>
+            <a:t> R$ 2.308,00 </a:t>
+          </a:fld>
+          <a:endParaRPr lang="en-US" sz="3600">
             <a:solidFill>
               <a:srgbClr val="00FF99"/>
             </a:solidFill>
@@ -26305,6 +26306,10 @@
       <c r="D12" s="14">
         <v>2308</v>
       </c>
+      <c r="G12" s="16">
+        <f>GETPIVOTDATA("Total Value",$C$9)</f>
+        <v>2308</v>
+      </c>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C14" s="13" t="s">
@@ -26439,8 +26444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{210F14EF-C0B7-459D-9E09-3130BA4314A6}">
   <dimension ref="A2:AC98"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="92" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="92" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="U15" sqref="U15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29338,8 +29343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{953EFA6A-D504-4E20-8AC3-4CB73941EF92}">
   <dimension ref="A3:AC146"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U30" sqref="U30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33642,6 +33647,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010001E48B58A68BE64E9120D347E3E06B3A" ma:contentTypeVersion="19" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="2f90046ec77328b7f86417d2e03b3d33">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="851b35d3-0456-4d6a-bc2f-da927e91d158" xmlns:ns3="19483571-f922-4e8e-9c1c-26f0a2252132" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c815006ac2d4f05ee97fdd57e40d8e38" ns2:_="" ns3:_="">
     <xsd:import namespace="851b35d3-0456-4d6a-bc2f-da927e91d158"/>
@@ -33896,7 +33910,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="851b35d3-0456-4d6a-bc2f-da927e91d158">
@@ -33907,16 +33921,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3B4D9D5-B351-46EB-A728-C3362FE437D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32608D25-EC36-42FE-A1DC-F778995A6799}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -33935,7 +33948,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFD3D529-BCD3-4ECD-9B2A-42924892FFCB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -33944,12 +33957,4 @@
     <ds:schemaRef ds:uri="19483571-f922-4e8e-9c1c-26f0a2252132"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3B4D9D5-B351-46EB-A728-C3362FE437D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>